<commit_message>
Container With Most Water Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F7D16-CD7C-A74D-ABBD-8B984EC537D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62F7D3F-A6BB-BD46-90D6-425A500142CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="124">
   <si>
     <t>Question Number</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>O(Coins*Target)</t>
+  </si>
+  <si>
+    <t>2 Pointer, while l&lt;r. Move pointer with lower height.</t>
   </si>
 </sst>
 </file>
@@ -768,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,8 +842,15 @@
       <c r="D3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">

</xml_diff>

<commit_message>
Longest Consecutive Sequence Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D1454F-D615-B745-AEBA-3F94590B8805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98544312-8869-8445-B025-AA380963A659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="129">
   <si>
     <t>Question Number</t>
   </si>
@@ -418,6 +418,9 @@
   </si>
   <si>
     <t>Sort intervals by start time, for each interval check if starts after previous ends, ends after previous, or is encompassed by previous. Extra space for answer.</t>
+  </si>
+  <si>
+    <t>Create set from nums. For each num check if previous num is in set. If not then check for consecutive numbers. This makes no duplicate sequences.</t>
   </si>
 </sst>
 </file>
@@ -784,7 +787,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1337,8 +1340,15 @@
       <c r="D29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">

</xml_diff>

<commit_message>
Find Minimum In Rotated Sorted Array Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448CCD28-EE6D-3945-A7AB-9836F4DCA1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9619306E-F68B-394E-89C0-3A6F181A51E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
+    <sheet name="Other" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="133">
   <si>
     <t>Question Number</t>
   </si>
@@ -427,6 +428,12 @@
   </si>
   <si>
     <t>O(N*M)?</t>
+  </si>
+  <si>
+    <t>Log(N)</t>
+  </si>
+  <si>
+    <t>if mid-1 &gt;mid or mid+1&lt;mid return mid/mid+1. Else check if l&lt;mid and move l to mid+1, else move r to mid-1.</t>
   </si>
 </sst>
 </file>
@@ -792,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,8 +955,15 @@
       <c r="D7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -1340,7 +1354,9 @@
       <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -2221,4 +2237,47 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE2CDC4-B1AF-994D-AFC7-4FFEDAC138A0}">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Product of Array Except Self Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9619306E-F68B-394E-89C0-3A6F181A51E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC83DAB-293D-7948-8788-C2AD30FC6FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="133">
   <si>
     <t>Question Number</t>
   </si>
@@ -352,9 +352,6 @@
     <t>Hard</t>
   </si>
   <si>
-    <t>Array, Binary Search</t>
-  </si>
-  <si>
     <t>n(n+1)/2 - sum(nums)</t>
   </si>
   <si>
@@ -434,6 +431,9 @@
   </si>
   <si>
     <t>if mid-1 &gt;mid or mid+1&lt;mid return mid/mid+1. Else check if l&lt;mid and move l to mid+1, else move r to mid-1.</t>
+  </si>
+  <si>
+    <t>Count product of array without 0s and num of 0s. If num 0s &gt;1, return all 0s. If a 0 and this num isnt 0 append 0. if num is 0 append product, else append product/number</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,7 +808,7 @@
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="133.33203125" customWidth="1"/>
+    <col min="6" max="6" width="140.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -874,7 +874,7 @@
         <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>82</v>
@@ -920,7 +920,7 @@
         <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>82</v>
@@ -959,10 +959,10 @@
         <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -973,13 +973,20 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -1005,7 +1012,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>76</v>
@@ -1037,7 +1044,7 @@
         <v>77</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>82</v>
@@ -1092,7 +1099,7 @@
         <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>82</v>
@@ -1147,7 +1154,7 @@
         <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>98</v>
@@ -1202,10 +1209,10 @@
         <v>77</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1280,7 +1287,7 @@
         <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>82</v>
@@ -1335,10 +1342,10 @@
         <v>77</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1376,7 +1383,7 @@
         <v>77</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>82</v>
@@ -1438,7 +1445,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>79</v>
@@ -1454,7 +1461,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>79</v>
@@ -1495,10 +1502,10 @@
         <v>77</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1518,10 +1525,10 @@
         <v>77</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1619,7 +1626,7 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>82</v>
@@ -1761,10 +1768,10 @@
         <v>77</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1800,7 +1807,7 @@
         <v>77</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>102</v>
@@ -1876,7 +1883,7 @@
         <v>77</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>82</v>
@@ -1899,7 +1906,7 @@
         <v>77</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>82</v>
@@ -1938,7 +1945,7 @@
         <v>77</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>82</v>
@@ -1993,7 +2000,7 @@
         <v>77</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>77</v>
@@ -2048,7 +2055,7 @@
         <v>77</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>82</v>
@@ -2243,7 +2250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE2CDC4-B1AF-994D-AFC7-4FFEDAC138A0}">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Design Add and Search Words Data Structure Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC83DAB-293D-7948-8788-C2AD30FC6FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E876D6F-D6FF-FE4D-B627-3AEE08492745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="134">
   <si>
     <t>Question Number</t>
   </si>
@@ -424,9 +424,6 @@
     <t>If out of bounds return 0, if end of path return 1, else return dp of down a square + dp of right a square. Use lru_cache for effencies.</t>
   </si>
   <si>
-    <t>O(N*M)?</t>
-  </si>
-  <si>
     <t>Log(N)</t>
   </si>
   <si>
@@ -434,6 +431,12 @@
   </si>
   <si>
     <t>Count product of array without 0s and num of 0s. If num 0s &gt;1, return all 0s. If a 0 and this num isnt 0 append 0. if num is 0 append product, else append product/number</t>
+  </si>
+  <si>
+    <t>Create TrieNode class. Add word like Implement Trie. Search if '.' for all children of node call</t>
+  </si>
+  <si>
+    <t>Add O(all letters of all words) SearchO(height) for no .</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,10 +962,10 @@
         <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,7 +985,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>82</v>
@@ -1212,7 +1215,7 @@
         <v>128</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -2019,8 +2022,15 @@
       <c r="D63" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="E63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2">

</xml_diff>

<commit_message>
Reverse Linked List Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E876D6F-D6FF-FE4D-B627-3AEE08492745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB172759-C0A0-D246-8C43-BB07BDF2EA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="135">
   <si>
     <t>Question Number</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Add O(all letters of all words) SearchO(height) for no .</t>
+  </si>
+  <si>
+    <t>Prev=None, cur=head. While cur: next = cur.next, cur.next=prev, prev=cur, cur=next. Return prev</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1646,7 +1649,7 @@
         <v>88</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -1662,10 +1665,17 @@
         <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">

</xml_diff>

<commit_message>
Top K Frequent Elements Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347A7783-B22F-5C4D-A26F-2F3EBA70F439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AE369A-6A68-1947-BF3A-0E7B613609FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="138">
   <si>
     <t>Question Number</t>
   </si>
@@ -443,6 +443,12 @@
   </si>
   <si>
     <t>Def function to count palandroms starting from center. Call function on each char in string and take sum of all results.</t>
+  </si>
+  <si>
+    <t>O(Nlog(k))</t>
+  </si>
+  <si>
+    <t>count occurance of each num in dictionary. Use priority qeue to pop top k elements by value.</t>
   </si>
 </sst>
 </file>
@@ -808,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1454,7 +1460,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>79</v>
@@ -1486,13 +1492,20 @@
         <v>67</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
@@ -1548,7 +1561,7 @@
         <v>71</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Subtree of Another Tree Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AE369A-6A68-1947-BF3A-0E7B613609FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07286EDA-1C47-AD45-9957-EE0A810E93F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="140">
   <si>
     <t>Question Number</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>count occurance of each num in dictionary. Use priority qeue to pop top k elements by value.</t>
+  </si>
+  <si>
+    <t>O(T*ST)</t>
+  </si>
+  <si>
+    <t>Function checks if each tree =  subtree recursively. Call sameTree function recursively on all nodes of tree.</t>
   </si>
 </sst>
 </file>
@@ -814,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2181,8 +2187,15 @@
       <c r="D70" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2">

</xml_diff>

<commit_message>
Maximum Product Subarray Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07286EDA-1C47-AD45-9957-EE0A810E93F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD8F353-D06A-F74C-B9F9-EC33B936AEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="141">
   <si>
     <t>Question Number</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>Function checks if each tree =  subtree recursively. Call sameTree function recursively on all nodes of tree.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For every element in array keep track of min and max product and update with each number, keep a global max to return. </t>
   </si>
 </sst>
 </file>
@@ -821,7 +824,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,8 +963,15 @@
       <c r="D6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">

</xml_diff>

<commit_message>
Longest Increasing Subsequence Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD8F353-D06A-F74C-B9F9-EC33B936AEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6172F-ABF3-9F4B-A455-6B25EAD2A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="143">
   <si>
     <t>Question Number</t>
   </si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t xml:space="preserve">For every element in array keep track of min and max product and update with each number, keep a global max to return. </t>
+  </si>
+  <si>
+    <t>DP map keep track of longest starting at end and if num is less than curr, update DP. Create array add first num, for remaining nums if num is higher than last add to array else replace last num in array. Can use Binary Search to speed up.</t>
+  </si>
+  <si>
+    <t>O(N^2) / O(nLog(N))</t>
   </si>
 </sst>
 </file>
@@ -824,7 +830,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1353,8 +1359,15 @@
       <c r="D26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -1868,7 +1881,9 @@
       <c r="C53" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>

</xml_diff>

<commit_message>
Decode Ways and Jump Game Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6172F-ABF3-9F4B-A455-6B25EAD2A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D8A4F4-745B-A34E-8A88-2907C0EF0633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="145">
   <si>
     <t>Question Number</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>O(N^2) / O(nLog(N))</t>
+  </si>
+  <si>
+    <t>for every num if it can be reached up longest with max of longest and num+jump distance. If num cant be reached return false. Return true if last node reached.</t>
+  </si>
+  <si>
+    <t>create array of ans, for every num add the answer to the problem of num before. If 9&lt;num and num before&lt;27 add answer of 2 before as well. Return last in array of answers.</t>
   </si>
 </sst>
 </file>
@@ -829,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1226,8 +1232,15 @@
       <c r="D19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -1288,8 +1301,15 @@
       <c r="D22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2">

</xml_diff>

<commit_message>
House robber 2 and Search in Rotat ed Sorted Array
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D8A4F4-745B-A34E-8A88-2907C0EF0633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64150B6B-6349-094B-A52A-D13DC1E637F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="148">
   <si>
     <t>Question Number</t>
   </si>
@@ -470,6 +470,15 @@
   </si>
   <si>
     <t>create array of ans, for every num add the answer to the problem of num before. If 9&lt;num and num before&lt;27 add answer of 2 before as well. Return last in array of answers.</t>
+  </si>
+  <si>
+    <t>O(log(n))</t>
+  </si>
+  <si>
+    <t>While l&lt;=r: if mid = target return. If l&lt;mid then check if target is in range of l and mid and change r. Else change l. Else check if target inbetween mid and r and change l else change r.</t>
+  </si>
+  <si>
+    <t>Do House Robber but take max between houses - first house and houses - last house</t>
   </si>
 </sst>
 </file>
@@ -836,7 +845,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1042,10 +1051,17 @@
         <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -1363,8 +1379,15 @@
       <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2">

</xml_diff>

<commit_message>
Merge k Sorted Lists Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64150B6B-6349-094B-A52A-D13DC1E637F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347E3214-2857-844E-9376-CF97313DDF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="149">
   <si>
     <t>Question Number</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>Do House Robber but take max between houses - first house and houses - last house</t>
+  </si>
+  <si>
+    <t>Divide and conquer using merge 2 sorted lists</t>
   </si>
 </sst>
 </file>
@@ -844,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1519,7 +1522,7 @@
         <v>92</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1675,7 +1678,7 @@
         <v>88</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>77</v>
@@ -1698,10 +1701,17 @@
         <v>88</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
@@ -2033,7 +2043,7 @@
         <v>91</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>

</xml_diff>

<commit_message>
Lowest Common Ancestor Of a Binary Search Tree Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F817468A-B319-0A49-B37D-DC1763506A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04972A2-8FA0-C14B-BD84-4E906721191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
   <si>
     <t>Question Number</t>
   </si>
@@ -355,9 +355,6 @@
     <t>n(n+1)/2 - sum(nums)</t>
   </si>
   <si>
-    <t>Set root.right to self.invertTree(root,left) and vica versa</t>
-  </si>
-  <si>
     <t>Array, Hashtable</t>
   </si>
   <si>
@@ -491,6 +488,15 @@
   </si>
   <si>
     <t>O(len(s)*DictWord)</t>
+  </si>
+  <si>
+    <t>Set root.right to self.invertTree(right,left) and vica versa</t>
+  </si>
+  <si>
+    <t>If q/p of different sides of root return root else move down. If root = p or q return p or q.</t>
+  </si>
+  <si>
+    <t>O(H)</t>
   </si>
 </sst>
 </file>
@@ -856,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,7 +937,7 @@
         <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>82</v>
@@ -977,7 +983,7 @@
         <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>82</v>
@@ -1000,7 +1006,7 @@
         <v>77</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>82</v>
@@ -1023,10 +1029,10 @@
         <v>77</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1046,7 +1052,7 @@
         <v>77</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>82</v>
@@ -1069,10 +1075,10 @@
         <v>77</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1083,7 +1089,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>76</v>
@@ -1115,7 +1121,7 @@
         <v>77</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>82</v>
@@ -1225,7 +1231,7 @@
         <v>77</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>98</v>
@@ -1264,7 +1270,7 @@
         <v>77</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>82</v>
@@ -1287,10 +1293,10 @@
         <v>77</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1333,7 +1339,7 @@
         <v>77</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>82</v>
@@ -1356,10 +1362,10 @@
         <v>77</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1379,7 +1385,7 @@
         <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>82</v>
@@ -1402,7 +1408,7 @@
         <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>82</v>
@@ -1425,10 +1431,10 @@
         <v>77</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1448,10 +1454,10 @@
         <v>77</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1489,7 +1495,7 @@
         <v>77</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>82</v>
@@ -1567,7 +1573,7 @@
         <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>79</v>
@@ -1583,7 +1589,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>79</v>
@@ -1592,10 +1598,10 @@
         <v>77</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1615,10 +1621,10 @@
         <v>77</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1638,10 +1644,10 @@
         <v>77</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -1661,10 +1667,10 @@
         <v>77</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -1730,10 +1736,10 @@
         <v>77</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1753,7 +1759,7 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>82</v>
@@ -1792,7 +1798,7 @@
         <v>77</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>82</v>
@@ -1902,10 +1908,10 @@
         <v>77</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1941,7 +1947,7 @@
         <v>77</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>102</v>
@@ -1980,7 +1986,7 @@
         <v>77</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>98</v>
@@ -2026,7 +2032,7 @@
         <v>77</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>82</v>
@@ -2049,7 +2055,7 @@
         <v>77</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>82</v>
@@ -2088,7 +2094,7 @@
         <v>77</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>82</v>
@@ -2143,7 +2149,7 @@
         <v>77</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>77</v>
@@ -2166,10 +2172,10 @@
         <v>77</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2205,7 +2211,7 @@
         <v>77</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>82</v>
@@ -2238,10 +2244,17 @@
         <v>91</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
@@ -2292,10 +2305,10 @@
         <v>77</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Longest Repeating Character Replacement Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04972A2-8FA0-C14B-BD84-4E906721191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C41180-E370-BF4A-886B-28775D738226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="155">
   <si>
     <t>Question Number</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>O(H)</t>
+  </si>
+  <si>
+    <t>Dict of freq of chars, keep l, r pointer. Move r constantly, add r char to freq, if freq-l+r+1&gt;k move l otherwise don’t, take max of ans and r-l+1.</t>
   </si>
 </sst>
 </file>
@@ -862,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,7 +1209,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>79</v>
@@ -1468,7 +1471,7 @@
         <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>79</v>
@@ -1486,7 +1489,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>79</v>
@@ -1966,8 +1969,15 @@
       <c r="D53" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2">

</xml_diff>

<commit_message>
Lowest Common Ancestor of a Binary Tree Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C41180-E370-BF4A-886B-28775D738226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5884DA81-A861-1445-905E-471487525AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="156">
   <si>
     <t>Question Number</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Dict of freq of chars, keep l, r pointer. Move r constantly, add r char to freq, if freq-l+r+1&gt;k move l otherwise don’t, take max of ans and r-l+1.</t>
+  </si>
+  <si>
+    <t>Use dfs, if node then check left and right trees if 2 of curr, left or right are targets then curr node is ans, else if one of them return true else return false. Use var to store ans with init.</t>
   </si>
 </sst>
 </file>
@@ -865,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2279,8 +2282,15 @@
       <c r="D68" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+      <c r="E68" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2">

</xml_diff>

<commit_message>
Number of Islands Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5884DA81-A861-1445-905E-471487525AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522DCA15-46F8-EC41-832A-9CD6C1F22D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="157">
   <si>
     <t>Question Number</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>Use dfs, if node then check left and right trees if 2 of curr, left or right are targets then curr node is ans, else if one of them return true else return false. Use var to store ans with init.</t>
+  </si>
+  <si>
+    <t>Use dfs on every point, if 1 and not in visited add an island and run dfs.</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,8 +1539,15 @@
       <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2">

</xml_diff>

<commit_message>
Binary Tree Level Order Traversal Complete
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Career/Interview Prep/Leetcode-Blind-75/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522DCA15-46F8-EC41-832A-9CD6C1F22D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DD6DEA-059E-F243-984C-B98ECDBF86FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
+    <workbookView xWindow="20000" yWindow="5900" windowWidth="28800" windowHeight="17500" xr2:uid="{A76C918A-9F74-8142-BCC6-CF8F109C8848}"/>
   </bookViews>
   <sheets>
     <sheet name="Blind 75" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="158">
   <si>
     <t>Question Number</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Use dfs on every point, if 1 and not in visited add an island and run dfs.</t>
+  </si>
+  <si>
+    <t>Use bfs but don’t update q with children until q is empty. Use separate array to store curr next and nextLevel</t>
   </si>
 </sst>
 </file>
@@ -871,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8E28F3-970E-0641-83D6-0B40B8CCDF83}">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2097,8 +2100,15 @@
       <c r="D58" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2">

</xml_diff>